<commit_message>
Added new product types to the example
</commit_message>
<xml_diff>
--- a/ExcelExamples/GeneralSwap.xlsx
+++ b/ExcelExamples/GeneralSwap.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="10290"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="10290" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Product And Value" sheetId="1" r:id="rId1"/>
-    <sheet name="Curves" sheetId="2" r:id="rId2"/>
+    <sheet name="Fixed CCIRS" sheetId="1" r:id="rId1"/>
+    <sheet name="Amortising Swap" sheetId="3" r:id="rId2"/>
+    <sheet name="FX Forward or FX Swap" sheetId="4" r:id="rId3"/>
+    <sheet name="Curves and Model" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621" calcMode="manual" calcOnSave="0"/>
+  <calcPr calcId="145621" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="51">
   <si>
     <t>name</t>
   </si>
@@ -71,9 +73,6 @@
     <t>fxForecastCurves</t>
   </si>
   <si>
-    <t>valueResults</t>
-  </si>
-  <si>
     <t>model</t>
   </si>
   <si>
@@ -111,14 +110,75 @@
   </si>
   <si>
     <t>QSA.Value</t>
+  </si>
+  <si>
+    <t>floatLeg</t>
+  </si>
+  <si>
+    <t>floatingIndex</t>
+  </si>
+  <si>
+    <t>JIBAR3M</t>
+  </si>
+  <si>
+    <t>resetDates</t>
+  </si>
+  <si>
+    <t>spreads</t>
+  </si>
+  <si>
+    <t>fixedLeg</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>ccirsValueResults</t>
+  </si>
+  <si>
+    <t>amortSwapValueResults</t>
+  </si>
+  <si>
+    <t>QSA.CreateFloatLeg</t>
+  </si>
+  <si>
+    <t>fxSwap</t>
+  </si>
+  <si>
+    <t>amounts</t>
+  </si>
+  <si>
+    <t>currencies</t>
+  </si>
+  <si>
+    <t>QSA.CreateCashLeg</t>
+  </si>
+  <si>
+    <t>fxSwapValueResults</t>
+  </si>
+  <si>
+    <t>discountCuve</t>
+  </si>
+  <si>
+    <t>floatingRateIndex</t>
+  </si>
+  <si>
+    <t>JIBAR6M</t>
+  </si>
+  <si>
+    <t>LIBOR3M</t>
+  </si>
+  <si>
+    <t>QSA.CreateRateForecastCurveFromDiscount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -143,7 +203,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,6 +234,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -188,7 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -200,7 +266,9 @@
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,15 +599,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J37"/>
+  <dimension ref="B2:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="60.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.125" bestFit="1" customWidth="1"/>
@@ -551,7 +619,7 @@
   <sheetData>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
@@ -849,109 +917,70 @@
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="str">
         <f>_xll.QSA.CreateFixedLeg(C3,C4,B7:B14,C7:C14,D7:D14,E7:E14)</f>
-        <v>fixedLegZAR0001.06:36:39-68</v>
+        <v>fixedLegZAR0001.08:29:00-70</v>
       </c>
       <c r="G16" s="6" t="str">
         <f>_xll.QSA.CreateFixedLeg(H3,H4,G7:G14,H7:H14,I7:I14,J7:J14)</f>
-        <v>fixedLegUSD0001.06:36:39-70</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B19" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>15</v>
+        <v>fixedLegUSD0001.08:29:00-71</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B20" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="10" t="str">
-        <f>Curves!B10</f>
-        <v>ZARDiscount.06:36:39-65</v>
+        <v>0</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
+      </c>
+      <c r="C22" s="10" t="str">
+        <f>B16</f>
+        <v>fixedLegZAR0001.08:29:00-70</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C23" s="10" t="str">
-        <f>Curves!L10</f>
-        <v>USDZARForwards.06:36:39-67</v>
+        <f>G16</f>
+        <v>fixedLegUSD0001.08:29:00-71</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="3">
+        <v>42636</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="6" t="str">
-        <f>_xll.QSA.CreateCurveModel(C20,C21,,C23)</f>
-        <v>curveModel.06:36:39-69</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B28" s="9" t="s">
-        <v>31</v>
+      <c r="B25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="10" t="str">
+        <f ca="1">'Curves and Model'!B28</f>
+        <v>curveModel.08:29:00-72</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="str">
+        <f ca="1">_xll.QSA.Value(C21,C22:C23,C24,C25)</f>
+        <v>ccirsValueResults.08:29:00-75</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="10" t="str">
-        <f>B16</f>
-        <v>fixedLegZAR0001.06:36:39-68</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C31" s="10" t="str">
-        <f>G16</f>
-        <v>fixedLegUSD0001.06:36:39-70</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="3">
-        <v>42636</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C33" s="10" t="str">
-        <f>B25</f>
-        <v>curveModel.06:36:39-69</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="6" t="str">
-        <f>_xll.QSA.Value(C29,C30:C31,C32,C33)</f>
-        <v>valueResults.06:36:39-71</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="11">
-        <f>_xll.QSA.GetResults(B35,"value")</f>
+        <v>37</v>
+      </c>
+      <c r="C29" s="12">
+        <f ca="1">_xll.QSA.GetResults(B27,"value")</f>
         <v>-179484.52557973986</v>
       </c>
     </row>
@@ -962,18 +991,549 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M10"/>
+  <dimension ref="B2:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="24.375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="7" max="7" width="5.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>42639</v>
+      </c>
+      <c r="C7" s="3">
+        <f>EDATE(B7,3)</f>
+        <v>42730</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+      <c r="F7" s="13">
+        <f>(C7-B7)/365</f>
+        <v>0.24931506849315069</v>
+      </c>
+      <c r="H7" s="2">
+        <f>-D7</f>
+        <v>-1000000</v>
+      </c>
+      <c r="I7" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <f>C7</f>
+        <v>42730</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" ref="C8:C14" si="0">EDATE(B8,3)</f>
+        <v>42820</v>
+      </c>
+      <c r="D8" s="2">
+        <f>D7-125000</f>
+        <v>875000</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="13">
+        <f t="shared" ref="F8:F14" si="1">(C8-B8)/365</f>
+        <v>0.24657534246575341</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" ref="H8:H14" si="2">-D8</f>
+        <v>-875000</v>
+      </c>
+      <c r="I8" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <f t="shared" ref="B9:B14" si="3">C8</f>
+        <v>42820</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>42912</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" ref="D9:D14" si="4">D8-125000</f>
+        <v>750000</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0</v>
+      </c>
+      <c r="F9" s="13">
+        <f t="shared" si="1"/>
+        <v>0.25205479452054796</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="2"/>
+        <v>-750000</v>
+      </c>
+      <c r="I9" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <f t="shared" si="3"/>
+        <v>42912</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>43004</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="4"/>
+        <v>625000</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+      <c r="F10" s="13">
+        <f t="shared" si="1"/>
+        <v>0.25205479452054796</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="2"/>
+        <v>-625000</v>
+      </c>
+      <c r="I10" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <f t="shared" si="3"/>
+        <v>43004</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="0"/>
+        <v>43095</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="4"/>
+        <v>500000</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0</v>
+      </c>
+      <c r="F11" s="13">
+        <f t="shared" si="1"/>
+        <v>0.24931506849315069</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="2"/>
+        <v>-500000</v>
+      </c>
+      <c r="I11" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <f t="shared" si="3"/>
+        <v>43095</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="0"/>
+        <v>43185</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="4"/>
+        <v>375000</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
+      <c r="F12" s="13">
+        <f t="shared" si="1"/>
+        <v>0.24657534246575341</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="2"/>
+        <v>-375000</v>
+      </c>
+      <c r="I12" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <f t="shared" si="3"/>
+        <v>43185</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="0"/>
+        <v>43277</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="4"/>
+        <v>250000</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0</v>
+      </c>
+      <c r="F13" s="13">
+        <f t="shared" si="1"/>
+        <v>0.25205479452054796</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="2"/>
+        <v>-250000</v>
+      </c>
+      <c r="I13" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <f t="shared" si="3"/>
+        <v>43277</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="0"/>
+        <v>43369</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="4"/>
+        <v>125000</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13">
+        <f t="shared" si="1"/>
+        <v>0.25205479452054796</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="2"/>
+        <v>-125000</v>
+      </c>
+      <c r="I14" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+    </row>
+    <row r="16" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="str">
+        <f>_xll.QSA.CreateFloatLeg(C2,C3,C4,B7:B14,C7:C14,D7:D14,E7:E14,F7:F14)</f>
+        <v>floatLeg.08:29:00-65</v>
+      </c>
+      <c r="I17" s="6" t="str">
+        <f>_xll.QSA.CreateFixedLeg(I2,I3,C7:C14,H7:H14,I7:I14,F7:F14)</f>
+        <v>fixedLeg.08:29:00-61</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B20" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="10" t="str">
+        <f>B17</f>
+        <v>floatLeg.08:29:00-65</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="10" t="str">
+        <f>I17</f>
+        <v>fixedLeg.08:29:00-61</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="3">
+        <v>42636</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="10" t="str">
+        <f ca="1">'Curves and Model'!B28</f>
+        <v>curveModel.08:29:00-72</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="str">
+        <f ca="1">_xll.QSA.Value(C21,C22:C23,C24,C25)</f>
+        <v>amortSwapValueResults.08:29:00-74</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="12">
+        <f ca="1">_xll.QSA.GetResults(B27,"value")</f>
+        <v>3341.7881313855064</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>42636</v>
+      </c>
+      <c r="C5" s="7">
+        <v>-13660000</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>42636</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>43001</v>
+      </c>
+      <c r="C7" s="7">
+        <v>14553000</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>43001</v>
+      </c>
+      <c r="C8" s="7">
+        <v>-1000000</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B11" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="str">
+        <f>_xll.QSA.CreateCashLeg(C2,B5:B8,C5:C8,D5:D8)</f>
+        <v>fxSwap.08:29:00-60</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B14" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="10" t="str">
+        <f>B12</f>
+        <v>fxSwap.08:29:00-60</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="3">
+        <v>42636</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="10" t="str">
+        <f ca="1">'Curves and Model'!B28</f>
+        <v>curveModel.08:29:00-72</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="str">
+        <f ca="1">_xll.QSA.Value(C15,C16,C18,C19)</f>
+        <v>fxSwapValueResults.08:29:00-73</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="12">
+        <f ca="1">_xll.QSA.GetResults(B21,"value")</f>
+        <v>341.00622510910034</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:M28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="28.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="31.375" bestFit="1" customWidth="1"/>
@@ -982,7 +1542,7 @@
   <sheetData>
     <row r="2" spans="2:13" ht="21" x14ac:dyDescent="0.35">
       <c r="L2" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
@@ -996,19 +1556,19 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="L3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
@@ -1028,10 +1588,10 @@
         <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>8</v>
@@ -1039,7 +1599,7 @@
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="L5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>2</v>
@@ -1065,7 +1625,7 @@
         <v>5</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M6" s="2">
         <v>13.66</v>
@@ -1091,11 +1651,11 @@
         <v>0.01</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M7" s="10" t="str">
         <f>H10</f>
-        <v>USDDiscountAndBasis.06:36:39-64</v>
+        <v>USDDiscountAndBasis.08:29:00-62</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
@@ -1118,29 +1678,154 @@
         <v>1.2E-2</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M8" s="10" t="str">
         <f>E10</f>
-        <v>ZARBasis.06:36:39-66</v>
+        <v>ZARBasis.08:29:00-64</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="str">
         <f>_xll.QSA.CreateDatesAndRatesCurve(C3,B7:B8,C7:C8,C4)</f>
-        <v>ZARDiscount.06:36:39-65</v>
+        <v>ZARDiscount.08:29:00-63</v>
       </c>
       <c r="E10" s="6" t="str">
         <f>_xll.QSA.CreateDatesAndRatesCurve(F3,E7:E8,F7:F8,F4)</f>
-        <v>ZARBasis.06:36:39-66</v>
+        <v>ZARBasis.08:29:00-64</v>
       </c>
       <c r="H10" s="6" t="str">
         <f>_xll.QSA.CreateDatesAndRatesCurve(I3,H7:H8,I7:I8,I4)</f>
-        <v>USDDiscountAndBasis.06:36:39-64</v>
+        <v>USDDiscountAndBasis.08:29:00-62</v>
       </c>
       <c r="L10" s="6" t="str">
         <f>_xll.QSA.CreateFXForecastCurve(M3,M4,M5,M6,M7,M8)</f>
-        <v>USDZARForwards.06:36:39-67</v>
+        <v>USDZARForwards.08:29:00-69</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="B13" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="str">
+        <f>"forecast"&amp;C15</f>
+        <v>forecastJIBAR3M</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="10" t="str">
+        <f>B10</f>
+        <v>ZARDiscount.08:29:00-63</v>
+      </c>
+      <c r="E15" s="6" t="str">
+        <f>_xll.QSA.CreateRateForecastCurveFromDiscount(B15,C15,D15)</f>
+        <v>forecastJIBAR3M.08:29:00-68</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="str">
+        <f t="shared" ref="B16:B17" si="0">"forecast"&amp;C16</f>
+        <v>forecastJIBAR6M</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="10" t="str">
+        <f>B10</f>
+        <v>ZARDiscount.08:29:00-63</v>
+      </c>
+      <c r="E16" s="6" t="str">
+        <f>_xll.QSA.CreateRateForecastCurveFromDiscount(B16,C16,D16)</f>
+        <v>forecastJIBAR6M.08:29:00-67</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>forecastLIBOR3M</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="10" t="str">
+        <f>H10</f>
+        <v>USDDiscountAndBasis.08:29:00-62</v>
+      </c>
+      <c r="E17" s="6" t="str">
+        <f>_xll.QSA.CreateRateForecastCurveFromDiscount(B17,C17,D17)</f>
+        <v>forecastLIBOR3M.08:29:00-66</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B20" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="10" t="str">
+        <f>'Curves and Model'!B10</f>
+        <v>ZARDiscount.08:29:00-63</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="10" t="str">
+        <f>E15</f>
+        <v>forecastJIBAR3M.08:29:00-68</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="10" t="str">
+        <f>E16</f>
+        <v>forecastJIBAR6M.08:29:00-67</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="10" t="str">
+        <f>E17</f>
+        <v>forecastLIBOR3M.08:29:00-66</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="10" t="str">
+        <f>'Curves and Model'!L10</f>
+        <v>USDZARForwards.08:29:00-69</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="str">
+        <f ca="1">_xll.QSA.CreateCurveModel(C21,C22,C23:C25,C26)</f>
+        <v>curveModel.08:29:34-76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working FRA with SA conventions for UJ teaching.
</commit_message>
<xml_diff>
--- a/ExcelExamples/GeneralSwap.xlsx
+++ b/ExcelExamples/GeneralSwap.xlsx
@@ -917,11 +917,11 @@
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="str">
         <f>_xll.QSA.CreateFixedLeg(C3,C4,B7:B14,C7:C14,D7:D14,E7:E14)</f>
-        <v>fixedLegZAR0001.08:29:00-70</v>
+        <v>fixedLegZAR0001.19:30:44-16</v>
       </c>
       <c r="G16" s="6" t="str">
         <f>_xll.QSA.CreateFixedLeg(H3,H4,G7:G14,H7:H14,I7:I14,J7:J14)</f>
-        <v>fixedLegUSD0001.08:29:00-71</v>
+        <v>fixedLegUSD0001.19:30:44-17</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="21" x14ac:dyDescent="0.35">
@@ -943,13 +943,13 @@
       </c>
       <c r="C22" s="10" t="str">
         <f>B16</f>
-        <v>fixedLegZAR0001.08:29:00-70</v>
+        <v>fixedLegZAR0001.19:30:44-16</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C23" s="10" t="str">
         <f>G16</f>
-        <v>fixedLegUSD0001.08:29:00-71</v>
+        <v>fixedLegUSD0001.19:30:44-17</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
@@ -965,14 +965,14 @@
         <v>18</v>
       </c>
       <c r="C25" s="10" t="str">
-        <f ca="1">'Curves and Model'!B28</f>
-        <v>curveModel.08:29:00-72</v>
+        <f>'Curves and Model'!B28</f>
+        <v>curveModel.19:30:44-18</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="str">
-        <f ca="1">_xll.QSA.Value(C21,C22:C23,C24,C25)</f>
-        <v>ccirsValueResults.08:29:00-75</v>
+        <f>_xll.QSA.Value(C21,C22:C23,C24,C25)</f>
+        <v>ccirsValueResults.19:30:44-20</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
@@ -980,7 +980,7 @@
         <v>37</v>
       </c>
       <c r="C29" s="12">
-        <f ca="1">_xll.QSA.GetResults(B27,"value")</f>
+        <f>_xll.QSA.GetResults(B27,"value")</f>
         <v>-179484.52557973986</v>
       </c>
     </row>
@@ -1300,11 +1300,11 @@
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="str">
         <f>_xll.QSA.CreateFloatLeg(C2,C3,C4,B7:B14,C7:C14,D7:D14,E7:E14,F7:F14)</f>
-        <v>floatLeg.08:29:00-65</v>
+        <v>floatLeg.19:30:44-10</v>
       </c>
       <c r="I17" s="6" t="str">
         <f>_xll.QSA.CreateFixedLeg(I2,I3,C7:C14,H7:H14,I7:I14,F7:F14)</f>
-        <v>fixedLeg.08:29:00-61</v>
+        <v>fixedLeg.19:30:44-8</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="21" x14ac:dyDescent="0.35">
@@ -1326,13 +1326,13 @@
       </c>
       <c r="C22" s="10" t="str">
         <f>B17</f>
-        <v>floatLeg.08:29:00-65</v>
+        <v>floatLeg.19:30:44-10</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C23" s="10" t="str">
         <f>I17</f>
-        <v>fixedLeg.08:29:00-61</v>
+        <v>fixedLeg.19:30:44-8</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
@@ -1348,14 +1348,14 @@
         <v>18</v>
       </c>
       <c r="C25" s="10" t="str">
-        <f ca="1">'Curves and Model'!B28</f>
-        <v>curveModel.08:29:00-72</v>
+        <f>'Curves and Model'!B28</f>
+        <v>curveModel.19:30:44-18</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="str">
-        <f ca="1">_xll.QSA.Value(C21,C22:C23,C24,C25)</f>
-        <v>amortSwapValueResults.08:29:00-74</v>
+        <f>_xll.QSA.Value(C21,C22:C23,C24,C25)</f>
+        <v>amortSwapValueResults.19:30:44-21</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
@@ -1363,7 +1363,7 @@
         <v>37</v>
       </c>
       <c r="C29" s="12">
-        <f ca="1">_xll.QSA.GetResults(B27,"value")</f>
+        <f>_xll.QSA.GetResults(B27,"value")</f>
         <v>3341.7881313855064</v>
       </c>
     </row>
@@ -1458,7 +1458,7 @@
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="str">
         <f>_xll.QSA.CreateCashLeg(C2,B5:B8,C5:C8,D5:D8)</f>
-        <v>fxSwap.08:29:00-60</v>
+        <v>fxSwap.19:30:44-5</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="21" x14ac:dyDescent="0.35">
@@ -1480,7 +1480,7 @@
       </c>
       <c r="C16" s="10" t="str">
         <f>B12</f>
-        <v>fxSwap.08:29:00-60</v>
+        <v>fxSwap.19:30:44-5</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -1496,14 +1496,14 @@
         <v>18</v>
       </c>
       <c r="C19" s="10" t="str">
-        <f ca="1">'Curves and Model'!B28</f>
-        <v>curveModel.08:29:00-72</v>
+        <f>'Curves and Model'!B28</f>
+        <v>curveModel.19:30:44-18</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="str">
-        <f ca="1">_xll.QSA.Value(C15,C16,C18,C19)</f>
-        <v>fxSwapValueResults.08:29:00-73</v>
+        <f>_xll.QSA.Value(C15,C16,C18,C19)</f>
+        <v>fxSwapValueResults.19:30:44-19</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
@@ -1511,7 +1511,7 @@
         <v>37</v>
       </c>
       <c r="C23" s="12">
-        <f ca="1">_xll.QSA.GetResults(B21,"value")</f>
+        <f>_xll.QSA.GetResults(B21,"value")</f>
         <v>341.00622510910034</v>
       </c>
     </row>
@@ -1655,7 +1655,7 @@
       </c>
       <c r="M7" s="10" t="str">
         <f>H10</f>
-        <v>USDDiscountAndBasis.08:29:00-62</v>
+        <v>USDDiscountAndBasis.19:30:44-11</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
@@ -1682,25 +1682,25 @@
       </c>
       <c r="M8" s="10" t="str">
         <f>E10</f>
-        <v>ZARBasis.08:29:00-64</v>
+        <v>ZARBasis.19:30:44-9</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="str">
         <f>_xll.QSA.CreateDatesAndRatesCurve(C3,B7:B8,C7:C8,C4)</f>
-        <v>ZARDiscount.08:29:00-63</v>
+        <v>ZARDiscount.19:30:44-7</v>
       </c>
       <c r="E10" s="6" t="str">
         <f>_xll.QSA.CreateDatesAndRatesCurve(F3,E7:E8,F7:F8,F4)</f>
-        <v>ZARBasis.08:29:00-64</v>
+        <v>ZARBasis.19:30:44-9</v>
       </c>
       <c r="H10" s="6" t="str">
         <f>_xll.QSA.CreateDatesAndRatesCurve(I3,H7:H8,I7:I8,I4)</f>
-        <v>USDDiscountAndBasis.08:29:00-62</v>
+        <v>USDDiscountAndBasis.19:30:44-11</v>
       </c>
       <c r="L10" s="6" t="str">
         <f>_xll.QSA.CreateFXForecastCurve(M3,M4,M5,M6,M7,M8)</f>
-        <v>USDZARForwards.08:29:00-69</v>
+        <v>USDZARForwards.19:30:44-12</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="21" x14ac:dyDescent="0.35">
@@ -1729,11 +1729,11 @@
       </c>
       <c r="D15" s="10" t="str">
         <f>B10</f>
-        <v>ZARDiscount.08:29:00-63</v>
+        <v>ZARDiscount.19:30:44-7</v>
       </c>
       <c r="E15" s="6" t="str">
         <f>_xll.QSA.CreateRateForecastCurveFromDiscount(B15,C15,D15)</f>
-        <v>forecastJIBAR3M.08:29:00-68</v>
+        <v>forecastJIBAR3M.19:30:44-15</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
@@ -1746,11 +1746,11 @@
       </c>
       <c r="D16" s="10" t="str">
         <f>B10</f>
-        <v>ZARDiscount.08:29:00-63</v>
+        <v>ZARDiscount.19:30:44-7</v>
       </c>
       <c r="E16" s="6" t="str">
         <f>_xll.QSA.CreateRateForecastCurveFromDiscount(B16,C16,D16)</f>
-        <v>forecastJIBAR6M.08:29:00-67</v>
+        <v>forecastJIBAR6M.19:30:44-14</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -1763,11 +1763,11 @@
       </c>
       <c r="D17" s="10" t="str">
         <f>H10</f>
-        <v>USDDiscountAndBasis.08:29:00-62</v>
+        <v>USDDiscountAndBasis.19:30:44-11</v>
       </c>
       <c r="E17" s="6" t="str">
         <f>_xll.QSA.CreateRateForecastCurveFromDiscount(B17,C17,D17)</f>
-        <v>forecastLIBOR3M.08:29:00-66</v>
+        <v>forecastLIBOR3M.19:30:44-13</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="21" x14ac:dyDescent="0.35">
@@ -1789,7 +1789,7 @@
       </c>
       <c r="C22" s="10" t="str">
         <f>'Curves and Model'!B10</f>
-        <v>ZARDiscount.08:29:00-63</v>
+        <v>ZARDiscount.19:30:44-7</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -1798,19 +1798,19 @@
       </c>
       <c r="C23" s="10" t="str">
         <f>E15</f>
-        <v>forecastJIBAR3M.08:29:00-68</v>
+        <v>forecastJIBAR3M.19:30:44-15</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C24" s="10" t="str">
         <f>E16</f>
-        <v>forecastJIBAR6M.08:29:00-67</v>
+        <v>forecastJIBAR6M.19:30:44-14</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C25" s="10" t="str">
         <f>E17</f>
-        <v>forecastLIBOR3M.08:29:00-66</v>
+        <v>forecastLIBOR3M.19:30:44-13</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
@@ -1819,13 +1819,13 @@
       </c>
       <c r="C26" s="10" t="str">
         <f>'Curves and Model'!L10</f>
-        <v>USDZARForwards.08:29:00-69</v>
+        <v>USDZARForwards.19:30:44-12</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="str">
-        <f ca="1">_xll.QSA.CreateCurveModel(C21,C22,C23:C25,C26)</f>
-        <v>curveModel.08:29:34-76</v>
+        <f>_xll.QSA.CreateCurveModel(C21,C22,C23:C25,C26)</f>
+        <v>curveModel.19:30:44-18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>